<commit_message>
Update the latest scores
</commit_message>
<xml_diff>
--- a/input/r16/world_cup_2018r16_Mo.xlsx
+++ b/input/r16/world_cup_2018r16_Mo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\wc2018\input\r16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moli/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91BCF1FE-481E-8D46-A7FD-53A372E2FBAB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14700" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29860" windowHeight="20440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T" sheetId="1" state="hidden" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <definedName name="T">T!$1:$1048576</definedName>
     <definedName name="teams">Settings!$I$17:$I$48</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -7791,16 +7792,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
-    <numFmt numFmtId="177" formatCode=";;;"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode=";;;"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7814,7 +7815,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7833,7 +7834,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -7870,7 +7871,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7883,7 +7884,7 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -7906,14 +7907,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7932,7 +7933,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -8925,7 +8926,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -8964,7 +8965,7 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
@@ -8988,7 +8989,7 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
@@ -9092,7 +9093,7 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
@@ -9108,7 +9109,7 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
@@ -9136,35 +9137,35 @@
       <alignment horizontal="right" vertical="center" indent="3" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -9319,91 +9320,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -9486,11 +9403,95 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="메모" xfId="2" builtinId="10"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="100">
     <dxf>
@@ -15453,7 +15454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15463,12 +15464,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -15602,7 +15603,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="81" t="s">
         <v>2074</v>
       </c>
@@ -15736,7 +15737,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
         <v>44</v>
       </c>
@@ -15870,7 +15871,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="81" t="s">
         <v>86</v>
       </c>
@@ -16004,7 +16005,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
         <v>129</v>
       </c>
@@ -16138,7 +16139,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="81" t="s">
         <v>170</v>
       </c>
@@ -16272,7 +16273,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="81" t="s">
         <v>209</v>
       </c>
@@ -16406,7 +16407,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
         <v>251</v>
       </c>
@@ -16540,7 +16541,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="81" t="s">
         <v>276</v>
       </c>
@@ -16674,7 +16675,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="81" t="s">
         <v>306</v>
       </c>
@@ -16808,7 +16809,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="81" t="s">
         <v>337</v>
       </c>
@@ -16942,7 +16943,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="81" t="s">
         <v>361</v>
       </c>
@@ -17076,7 +17077,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" s="81" t="s">
         <v>307</v>
       </c>
@@ -17210,7 +17211,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" s="81" t="s">
         <v>401</v>
       </c>
@@ -17344,7 +17345,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A15" s="81" t="s">
         <v>441</v>
       </c>
@@ -17478,7 +17479,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" s="81" t="s">
         <v>470</v>
       </c>
@@ -17612,7 +17613,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" s="81" t="s">
         <v>501</v>
       </c>
@@ -17746,7 +17747,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" s="81" t="s">
         <v>533</v>
       </c>
@@ -17880,7 +17881,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A21" s="81" t="s">
         <v>567</v>
       </c>
@@ -18014,7 +18015,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A22" s="81" t="s">
         <v>601</v>
       </c>
@@ -18148,7 +18149,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A23" s="81" t="s">
         <v>635</v>
       </c>
@@ -18282,7 +18283,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A24" s="81" t="s">
         <v>668</v>
       </c>
@@ -18416,7 +18417,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A25" s="81" t="s">
         <v>700</v>
       </c>
@@ -18550,7 +18551,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A26" s="81" t="s">
         <v>726</v>
       </c>
@@ -18684,7 +18685,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" s="81" t="s">
         <v>534</v>
       </c>
@@ -18818,7 +18819,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A28" s="81" t="s">
         <v>770</v>
       </c>
@@ -18952,7 +18953,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A29" s="81" t="s">
         <v>794</v>
       </c>
@@ -19086,7 +19087,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A30" s="81" t="s">
         <v>819</v>
       </c>
@@ -19220,7 +19221,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A31" s="81" t="s">
         <v>848</v>
       </c>
@@ -19354,7 +19355,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A32" s="81" t="s">
         <v>876</v>
       </c>
@@ -19488,7 +19489,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A33" s="81" t="s">
         <v>903</v>
       </c>
@@ -19622,7 +19623,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A34" s="81" t="s">
         <v>928</v>
       </c>
@@ -19756,7 +19757,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A35" s="81" t="s">
         <v>952</v>
       </c>
@@ -19890,7 +19891,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A36" s="81" t="s">
         <v>977</v>
       </c>
@@ -20024,7 +20025,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A37" s="81" t="s">
         <v>1004</v>
       </c>
@@ -20158,7 +20159,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A38" s="81" t="s">
         <v>1039</v>
       </c>
@@ -20292,7 +20293,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A39" s="81" t="s">
         <v>1075</v>
       </c>
@@ -20426,7 +20427,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A40" s="81" t="s">
         <v>1100</v>
       </c>
@@ -20560,7 +20561,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A41" s="81" t="s">
         <v>1120</v>
       </c>
@@ -20694,7 +20695,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A42" s="81" t="s">
         <v>1151</v>
       </c>
@@ -20828,7 +20829,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A43" s="81" t="s">
         <v>1172</v>
       </c>
@@ -20962,7 +20963,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A44" s="81" t="s">
         <v>1195</v>
       </c>
@@ -21096,7 +21097,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A45" s="81" t="s">
         <v>2171</v>
       </c>
@@ -21230,7 +21231,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A46" s="81" t="s">
         <v>1232</v>
       </c>
@@ -21364,7 +21365,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A47" s="81" t="s">
         <v>2167</v>
       </c>
@@ -21498,7 +21499,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A48" s="81" t="s">
         <v>2164</v>
       </c>
@@ -21632,7 +21633,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A49" s="81" t="s">
         <v>1263</v>
       </c>
@@ -21766,7 +21767,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A50" s="81" t="s">
         <v>1294</v>
       </c>
@@ -21900,7 +21901,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A51" s="81" t="s">
         <v>1329</v>
       </c>
@@ -22034,7 +22035,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A52" s="81" t="s">
         <v>1359</v>
       </c>
@@ -22168,7 +22169,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A53" s="81" t="s">
         <v>2165</v>
       </c>
@@ -22302,7 +22303,7 @@
         <v>2317</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A54" s="81" t="s">
         <v>2168</v>
       </c>
@@ -22436,7 +22437,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A55" s="81" t="s">
         <v>1385</v>
       </c>
@@ -22570,7 +22571,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A56" s="81" t="s">
         <v>1407</v>
       </c>
@@ -22704,7 +22705,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A57" s="81" t="s">
         <v>2166</v>
       </c>
@@ -22838,7 +22839,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A58" s="81" t="s">
         <v>2172</v>
       </c>
@@ -22972,7 +22973,7 @@
         <v>2404</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A59" s="81" t="s">
         <v>2170</v>
       </c>
@@ -23106,7 +23107,7 @@
         <v>2423</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A60" s="81" t="s">
         <v>2162</v>
       </c>
@@ -23240,7 +23241,7 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A61" s="81" t="s">
         <v>1436</v>
       </c>
@@ -23374,7 +23375,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A62" s="81" t="s">
         <v>1455</v>
       </c>
@@ -23508,7 +23509,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A63" s="81" t="s">
         <v>1485</v>
       </c>
@@ -23642,7 +23643,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A64" s="81" t="s">
         <v>2163</v>
       </c>
@@ -23776,7 +23777,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A65" s="81" t="s">
         <v>1514</v>
       </c>
@@ -23910,7 +23911,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A66" s="81" t="s">
         <v>1539</v>
       </c>
@@ -24044,7 +24045,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A67" s="81" t="s">
         <v>1575</v>
       </c>
@@ -24178,7 +24179,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A68" s="81" t="s">
         <v>2169</v>
       </c>
@@ -24312,7 +24313,7 @@
         <v>2504</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A69" s="81" t="s">
         <v>2161</v>
       </c>
@@ -24446,7 +24447,7 @@
         <v>2543</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A70" s="81" t="s">
         <v>1612</v>
       </c>
@@ -24580,7 +24581,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A71" s="81" t="s">
         <v>1618</v>
       </c>
@@ -24714,7 +24715,7 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A72" s="81" t="s">
         <v>1624</v>
       </c>
@@ -24848,7 +24849,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A73" s="81" t="s">
         <v>1630</v>
       </c>
@@ -24982,7 +24983,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A74" s="81" t="s">
         <v>1636</v>
       </c>
@@ -25116,7 +25117,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A75" s="81" t="s">
         <v>1644</v>
       </c>
@@ -25250,7 +25251,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A76" s="81" t="s">
         <v>1652</v>
       </c>
@@ -25384,7 +25385,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A77" s="81" t="s">
         <v>1659</v>
       </c>
@@ -25518,7 +25519,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A78" s="81" t="s">
         <v>1666</v>
       </c>
@@ -25652,7 +25653,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A79" s="81" t="s">
         <v>1673</v>
       </c>
@@ -25786,7 +25787,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A80" s="81" t="s">
         <v>1680</v>
       </c>
@@ -25920,7 +25921,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A81" s="81" t="s">
         <v>1687</v>
       </c>
@@ -26054,7 +26055,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A82" s="81" t="s">
         <v>1694</v>
       </c>
@@ -26188,7 +26189,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A83" s="81" t="s">
         <v>1702</v>
       </c>
@@ -26322,7 +26323,7 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A84" s="81" t="s">
         <v>1710</v>
       </c>
@@ -26456,7 +26457,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A85" s="81" t="s">
         <v>1717</v>
       </c>
@@ -26590,7 +26591,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A86" s="81" t="s">
         <v>1723</v>
       </c>
@@ -26724,7 +26725,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A87" s="81" t="s">
         <v>1743</v>
       </c>
@@ -26858,7 +26859,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A88" s="81" t="s">
         <v>1763</v>
       </c>
@@ -26992,7 +26993,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A89" s="81" t="s">
         <v>1783</v>
       </c>
@@ -27126,7 +27127,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A90" s="81" t="s">
         <v>1803</v>
       </c>
@@ -27260,7 +27261,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A91" s="81" t="s">
         <v>1823</v>
       </c>
@@ -27394,7 +27395,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A92" s="81" t="s">
         <v>1843</v>
       </c>
@@ -27528,7 +27529,7 @@
         <v>1843</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A93" s="81" t="s">
         <v>1863</v>
       </c>
@@ -27662,7 +27663,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A94" s="81" t="s">
         <v>1883</v>
       </c>
@@ -27796,7 +27797,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A95" s="81" t="s">
         <v>1903</v>
       </c>
@@ -27930,7 +27931,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A96" s="81" t="s">
         <v>1923</v>
       </c>
@@ -28064,7 +28065,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A97" s="81" t="s">
         <v>1943</v>
       </c>
@@ -28198,7 +28199,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A98" s="81" t="s">
         <v>1963</v>
       </c>
@@ -28332,7 +28333,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A99" s="81" t="s">
         <v>1983</v>
       </c>
@@ -28466,7 +28467,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A100" s="81" t="s">
         <v>1973</v>
       </c>
@@ -28600,7 +28601,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A101" s="81" t="s">
         <v>1993</v>
       </c>
@@ -28734,7 +28735,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A102" s="81" t="s">
         <v>2185</v>
       </c>
@@ -28868,43 +28869,43 @@
         <v>2223</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A103" s="82"/>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A104" s="82"/>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A105" s="82"/>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A106" s="82"/>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A107" s="82"/>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A108" s="82"/>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A109" s="82"/>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A110" s="82"/>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A111" s="82"/>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A112" s="82"/>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A113" s="82"/>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A114" s="82"/>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A115" s="81" t="s">
         <v>2032</v>
       </c>
@@ -29043,29 +29044,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I49"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="18.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="11"/>
-    <col min="5" max="5" width="1.125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="11"/>
+    <col min="1" max="1" width="1.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="11"/>
+    <col min="5" max="5" width="1.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="11"/>
     <col min="7" max="7" width="27.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="1.125" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="11"/>
+    <col min="8" max="8" width="2.6640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="83" t="s">
         <v>2114</v>
       </c>
@@ -29077,7 +29078,7 @@
       <c r="G2" s="84"/>
       <c r="H2" s="85"/>
     </row>
-    <row r="3" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="86"/>
       <c r="C3" s="87"/>
       <c r="D3" s="88"/>
@@ -29085,7 +29086,7 @@
       <c r="G3" s="87"/>
       <c r="H3" s="88"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="98" t="s">
         <v>2116</v>
       </c>
@@ -29097,7 +29098,7 @@
       <c r="G4" s="89"/>
       <c r="H4" s="88"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="86"/>
       <c r="C5" s="87"/>
       <c r="D5" s="88"/>
@@ -29109,7 +29110,7 @@
       </c>
       <c r="H5" s="88"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="98" t="s">
         <v>2119</v>
       </c>
@@ -29125,7 +29126,7 @@
       </c>
       <c r="H6" s="88"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="86"/>
       <c r="C7" s="87"/>
       <c r="D7" s="88"/>
@@ -29137,7 +29138,7 @@
       </c>
       <c r="H7" s="88"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="98" t="s">
         <v>2124</v>
       </c>
@@ -29153,7 +29154,7 @@
       </c>
       <c r="H8" s="88"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="86"/>
       <c r="C9" s="87"/>
       <c r="D9" s="88"/>
@@ -29165,7 +29166,7 @@
       </c>
       <c r="H9" s="88"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="98" t="s">
         <v>2130</v>
       </c>
@@ -29177,7 +29178,7 @@
       <c r="G10" s="94"/>
       <c r="H10" s="88"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="86"/>
       <c r="C11" s="87"/>
       <c r="D11" s="88"/>
@@ -29185,7 +29186,7 @@
       <c r="G11" s="96"/>
       <c r="H11" s="97"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="98" t="s">
         <v>2184</v>
       </c>
@@ -29194,13 +29195,13 @@
       </c>
       <c r="D12" s="88"/>
     </row>
-    <row r="13" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="95"/>
       <c r="C13" s="96"/>
       <c r="D13" s="97"/>
     </row>
-    <row r="14" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="99"/>
       <c r="C15" s="100"/>
       <c r="D15" s="101"/>
@@ -29217,7 +29218,7 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="86"/>
       <c r="C16" s="102" t="s">
         <v>2129</v>
@@ -29233,7 +29234,7 @@
       <c r="H16" s="108"/>
       <c r="I16" s="108"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="103" t="str">
         <f>VLOOKUP("Germany",T,lang,FALSE)</f>
         <v>Germany</v>
@@ -29249,7 +29250,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="103" t="str">
         <f>VLOOKUP("Brazil",T,lang,FALSE)</f>
         <v>Brazil</v>
@@ -29269,7 +29270,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="103" t="str">
         <f>VLOOKUP("Portugal",T,lang,FALSE)</f>
         <v>Portugal</v>
@@ -29289,7 +29290,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="103" t="str">
         <f>VLOOKUP("Argentina",T,lang,FALSE)</f>
         <v>Argentina</v>
@@ -29309,7 +29310,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="103" t="str">
         <f>VLOOKUP("Belgium",T,lang,FALSE)</f>
         <v>Belgium</v>
@@ -29329,7 +29330,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="103" t="str">
         <f>VLOOKUP("Spain",T,lang,FALSE)</f>
         <v>Spain</v>
@@ -29349,7 +29350,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="103" t="str">
         <f>VLOOKUP("Poland",T,lang,FALSE)</f>
         <v>Poland</v>
@@ -29369,7 +29370,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="103" t="str">
         <f>VLOOKUP("Switzerland",T,lang,FALSE)</f>
         <v>Switzerland</v>
@@ -29389,7 +29390,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="103" t="str">
         <f>VLOOKUP("France",T,lang,FALSE)</f>
         <v>France</v>
@@ -29409,7 +29410,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="103" t="str">
         <f>VLOOKUP("Peru",T,lang,FALSE)</f>
         <v>Peru</v>
@@ -29429,7 +29430,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="103" t="str">
         <f>VLOOKUP("Denmark",T,lang,FALSE)</f>
         <v>Denmark</v>
@@ -29449,7 +29450,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="103" t="str">
         <f>VLOOKUP("Colombia",T,lang,FALSE)</f>
         <v>Colombia</v>
@@ -29469,7 +29470,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="103" t="str">
         <f>VLOOKUP("England",T,lang,FALSE)</f>
         <v>England</v>
@@ -29489,7 +29490,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="103" t="str">
         <f>VLOOKUP("Mexico",T,lang,FALSE)</f>
         <v>Mexico</v>
@@ -29509,7 +29510,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="103" t="str">
         <f>VLOOKUP("Croatia",T,lang,FALSE)</f>
         <v>Croatia</v>
@@ -29529,7 +29530,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="103" t="str">
         <f>VLOOKUP("Sweden",T,lang,FALSE)</f>
         <v>Sweden</v>
@@ -29549,7 +29550,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="103" t="str">
         <f>VLOOKUP("Uruguay",T,lang,FALSE)</f>
         <v>Uruguay</v>
@@ -29569,7 +29570,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="103" t="str">
         <f>VLOOKUP("Iceland",T,lang,FALSE)</f>
         <v>Iceland</v>
@@ -29589,7 +29590,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="103" t="str">
         <f>VLOOKUP("Senegal",T,lang,FALSE)</f>
         <v>Senegal</v>
@@ -29609,7 +29610,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="103" t="str">
         <f>VLOOKUP("Costa Rica",T,lang,FALSE)</f>
         <v>Costa Rica</v>
@@ -29629,7 +29630,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="103" t="str">
         <f>VLOOKUP("Tunisia",T,lang,FALSE)</f>
         <v>Tunisia</v>
@@ -29649,7 +29650,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="103" t="str">
         <f>VLOOKUP("Egypt",T,lang,FALSE)</f>
         <v>Egypt</v>
@@ -29669,7 +29670,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="103" t="str">
         <f>VLOOKUP("Iran",T,lang,FALSE)</f>
         <v>Iran</v>
@@ -29689,7 +29690,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="103" t="str">
         <f>VLOOKUP("Serbia",T,lang,FALSE)</f>
         <v>Serbia</v>
@@ -29709,7 +29710,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="103" t="str">
         <f>VLOOKUP("Australia",T,lang,FALSE)</f>
         <v>Australia</v>
@@ -29729,7 +29730,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="103" t="str">
         <f>VLOOKUP("Morocco",T,lang,FALSE)</f>
         <v>Morocco</v>
@@ -29745,7 +29746,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="103" t="str">
         <f>VLOOKUP("Nigeria",T,lang,FALSE)</f>
         <v>Nigeria</v>
@@ -29765,7 +29766,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="103" t="str">
         <f>VLOOKUP("Panama",T,lang,FALSE)</f>
         <v>Panama</v>
@@ -29785,7 +29786,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="103" t="str">
         <f>VLOOKUP("Japan",T,lang,FALSE)</f>
         <v>Japan</v>
@@ -29805,7 +29806,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="103" t="str">
         <f>VLOOKUP("Korea Republic",T,lang,FALSE)</f>
         <v>Korea Republic</v>
@@ -29825,7 +29826,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="103" t="str">
         <f>VLOOKUP("Saudi Arabia",T,lang,FALSE)</f>
         <v>Saudi Arabia</v>
@@ -29841,7 +29842,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="103" t="str">
         <f>VLOOKUP("Russia",T,lang,FALSE)</f>
         <v>Russia</v>
@@ -29862,7 +29863,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="95"/>
       <c r="C49" s="96"/>
       <c r="D49" s="97"/>
@@ -29874,19 +29875,19 @@
   </sortState>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Language" prompt="Use drop-down List" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Language" prompt="Use drop-down List" sqref="C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>lang_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Summer Time" prompt="Use drop-down List" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Summer Time" prompt="Use drop-down List" sqref="C6" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select GTM-time" prompt="Use drop-down List" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select GTM-time" prompt="Use drop-down List" sqref="C8" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$F$18:$F$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Minutes" prompt="Use drop-down List" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Minutes" prompt="Use drop-down List" sqref="C10" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>$F$43:$F$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Your Favorite Team" prompt="Use drop-down List" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Your Favorite Team" prompt="Use drop-down List" sqref="C12" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>teams</formula1>
     </dataValidation>
   </dataValidations>
@@ -29896,87 +29897,87 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H11" workbookViewId="0">
-      <selection activeCell="BS36" sqref="BS36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="BG36" sqref="BG36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="22.5" style="6" customWidth="1"/>
-    <col min="6" max="7" width="4.375" style="7" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="7" customWidth="1"/>
     <col min="8" max="8" width="22.5" style="8" customWidth="1"/>
     <col min="9" max="9" width="3.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="14" style="9" customWidth="1"/>
     <col min="11" max="14" width="5.5" style="10" customWidth="1"/>
-    <col min="15" max="15" width="7.625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="6.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="10" customWidth="1"/>
     <col min="17" max="17" width="3.5" style="2" customWidth="1"/>
     <col min="18" max="18" width="15.5" style="58" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="16" style="65" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="5" style="59" hidden="1" customWidth="1"/>
-    <col min="22" max="25" width="6.125" style="58" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="4.375" style="59" hidden="1" customWidth="1"/>
+    <col min="22" max="25" width="6.1640625" style="58" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="4.33203125" style="59" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="5.5" style="58" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="13.5" style="59" hidden="1" customWidth="1"/>
     <col min="29" max="33" width="5.5" style="58" hidden="1" customWidth="1"/>
     <col min="34" max="36" width="6" style="58" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="5.5" style="58" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="6" style="58" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="7.125" style="59" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="7.1640625" style="59" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="10" style="59" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="15.375" style="60" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="4.625" style="61" hidden="1" customWidth="1"/>
-    <col min="43" max="46" width="4.625" style="62" hidden="1" customWidth="1"/>
-    <col min="47" max="49" width="9.125" style="63" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="9.125" style="64" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="3.375" style="3" customWidth="1"/>
-    <col min="52" max="52" width="19.625" style="3" customWidth="1"/>
+    <col min="41" max="41" width="15.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="4.6640625" style="61" hidden="1" customWidth="1"/>
+    <col min="43" max="46" width="4.6640625" style="62" hidden="1" customWidth="1"/>
+    <col min="47" max="49" width="9.1640625" style="63" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="9.1640625" style="64" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="3.33203125" style="3" customWidth="1"/>
+    <col min="52" max="52" width="19.6640625" style="3" customWidth="1"/>
     <col min="53" max="54" width="3" style="3" customWidth="1"/>
     <col min="55" max="56" width="2" style="3" customWidth="1"/>
-    <col min="57" max="57" width="3.375" style="3" customWidth="1"/>
-    <col min="58" max="58" width="19.625" style="3" customWidth="1"/>
+    <col min="57" max="57" width="3.33203125" style="3" customWidth="1"/>
+    <col min="58" max="58" width="19.6640625" style="3" customWidth="1"/>
     <col min="59" max="60" width="3" style="3" customWidth="1"/>
     <col min="61" max="62" width="2" style="3" customWidth="1"/>
-    <col min="63" max="63" width="3.375" style="3" customWidth="1"/>
-    <col min="64" max="64" width="19.625" style="3" customWidth="1"/>
+    <col min="63" max="63" width="3.33203125" style="3" customWidth="1"/>
+    <col min="64" max="64" width="19.6640625" style="3" customWidth="1"/>
     <col min="65" max="66" width="3" style="3" customWidth="1"/>
     <col min="67" max="68" width="2" style="3" customWidth="1"/>
-    <col min="69" max="69" width="3.375" style="3" customWidth="1"/>
-    <col min="70" max="70" width="19.625" style="3" customWidth="1"/>
+    <col min="69" max="69" width="3.33203125" style="3" customWidth="1"/>
+    <col min="70" max="70" width="19.6640625" style="3" customWidth="1"/>
     <col min="71" max="72" width="3" style="3" customWidth="1"/>
-    <col min="73" max="16384" width="8.875" style="3"/>
+    <col min="73" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="str">
+    <row r="1" spans="1:72" ht="47" x14ac:dyDescent="0.2">
+      <c r="A1" s="115" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30000,7 +30001,7 @@
       <c r="AS1" s="63"/>
       <c r="AT1" s="63"/>
     </row>
-    <row r="2" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S2" s="58"/>
       <c r="T2" s="58"/>
       <c r="U2" s="58"/>
@@ -30024,7 +30025,7 @@
       <c r="AS2" s="63"/>
       <c r="AT2" s="63"/>
     </row>
-    <row r="3" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -30039,11 +30040,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="116" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="116"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30067,45 +30068,45 @@
       <c r="AS3" s="63"/>
       <c r="AT3" s="63"/>
     </row>
-    <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138" t="str">
+    <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="117" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
+      <c r="J5" s="123" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="125"/>
     </row>
-    <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+    <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="120"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="128"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30169,36 +30170,36 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="109" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="131"/>
-      <c r="BA6" s="131"/>
-      <c r="BB6" s="132"/>
-      <c r="BE6" s="130" t="str">
+      <c r="AZ6" s="110"/>
+      <c r="BA6" s="110"/>
+      <c r="BB6" s="111"/>
+      <c r="BE6" s="109" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="131"/>
-      <c r="BG6" s="131"/>
-      <c r="BH6" s="132"/>
-      <c r="BK6" s="130" t="str">
+      <c r="BF6" s="110"/>
+      <c r="BG6" s="110"/>
+      <c r="BH6" s="111"/>
+      <c r="BK6" s="109" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="131"/>
-      <c r="BN6" s="132"/>
-      <c r="BQ6" s="130" t="str">
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="110"/>
+      <c r="BN6" s="111"/>
+      <c r="BQ6" s="109" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
+      <c r="BR6" s="110"/>
+      <c r="BS6" s="110"/>
+      <c r="BT6" s="111"/>
     </row>
-    <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>1</v>
       </c>
@@ -30260,24 +30261,24 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="134"/>
-      <c r="BA7" s="134"/>
-      <c r="BB7" s="135"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="134"/>
-      <c r="BG7" s="134"/>
-      <c r="BH7" s="135"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="134"/>
-      <c r="BN7" s="135"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
+      <c r="AY7" s="112"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="114"/>
+      <c r="BE7" s="112"/>
+      <c r="BF7" s="113"/>
+      <c r="BG7" s="113"/>
+      <c r="BH7" s="114"/>
+      <c r="BK7" s="112"/>
+      <c r="BL7" s="113"/>
+      <c r="BM7" s="113"/>
+      <c r="BN7" s="114"/>
+      <c r="BQ7" s="112"/>
+      <c r="BR7" s="113"/>
+      <c r="BS7" s="113"/>
+      <c r="BT7" s="114"/>
     </row>
-    <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>2</v>
       </c>
@@ -30459,7 +30460,7 @@
       <c r="BS8" s="25"/>
       <c r="BT8" s="25"/>
     </row>
-    <row r="9" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>3</v>
       </c>
@@ -30655,7 +30656,7 @@
       <c r="BS9" s="25"/>
       <c r="BT9" s="25"/>
     </row>
-    <row r="10" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>4</v>
       </c>
@@ -30821,7 +30822,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="118">
+      <c r="AY10" s="129">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -30851,7 +30852,7 @@
       <c r="BS10" s="25"/>
       <c r="BT10" s="25"/>
     </row>
-    <row r="11" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>5</v>
       </c>
@@ -31017,7 +31018,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="119"/>
+      <c r="AY11" s="130"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>Portugal</v>
@@ -31048,7 +31049,7 @@
       <c r="BS11" s="25"/>
       <c r="BT11" s="25"/>
     </row>
-    <row r="12" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>6</v>
       </c>
@@ -31200,7 +31201,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="118">
+      <c r="BE12" s="129">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31208,7 +31209,7 @@
         <v>Portugal</v>
       </c>
       <c r="BG12" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH12" s="30"/>
       <c r="BI12" s="25"/>
@@ -31224,7 +31225,7 @@
       <c r="BS12" s="25"/>
       <c r="BT12" s="25"/>
     </row>
-    <row r="13" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>7</v>
       </c>
@@ -31310,13 +31311,13 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="119"/>
+      <c r="BE13" s="130"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>France</v>
       </c>
       <c r="BG13" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH13" s="33"/>
       <c r="BI13" s="34"/>
@@ -31332,7 +31333,7 @@
       <c r="BS13" s="25"/>
       <c r="BT13" s="25"/>
     </row>
-    <row r="14" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>8</v>
       </c>
@@ -31502,7 +31503,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="118">
+      <c r="AY14" s="129">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31532,7 +31533,7 @@
       <c r="BS14" s="25"/>
       <c r="BT14" s="25"/>
     </row>
-    <row r="15" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>9</v>
       </c>
@@ -31702,7 +31703,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="119"/>
+      <c r="AY15" s="130"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>Argentina</v>
@@ -31733,7 +31734,7 @@
       <c r="BS15" s="25"/>
       <c r="BT15" s="25"/>
     </row>
-    <row r="16" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>10</v>
       </c>
@@ -31911,12 +31912,12 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="118">
+      <c r="BK16" s="129">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
         <f>T69</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="BM16" s="29">
         <v>1</v>
@@ -31929,7 +31930,7 @@
       <c r="BS16" s="25"/>
       <c r="BT16" s="25"/>
     </row>
-    <row r="17" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>11</v>
       </c>
@@ -32110,7 +32111,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="119"/>
+      <c r="BK17" s="130"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>Brazil</v>
@@ -32126,7 +32127,7 @@
       <c r="BS17" s="25"/>
       <c r="BT17" s="25"/>
     </row>
-    <row r="18" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>12</v>
       </c>
@@ -32272,7 +32273,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="118">
+      <c r="AY18" s="129">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32302,7 +32303,7 @@
       <c r="BS18" s="25"/>
       <c r="BT18" s="25"/>
     </row>
-    <row r="19" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>13</v>
       </c>
@@ -32379,7 +32380,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="119"/>
+      <c r="AY19" s="130"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>Mexico</v>
@@ -32410,7 +32411,7 @@
       <c r="BS19" s="25"/>
       <c r="BT19" s="25"/>
     </row>
-    <row r="20" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>14</v>
       </c>
@@ -32586,7 +32587,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="118">
+      <c r="BE20" s="129">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32610,7 +32611,7 @@
       <c r="BS20" s="25"/>
       <c r="BT20" s="25"/>
     </row>
-    <row r="21" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>15</v>
       </c>
@@ -32789,7 +32790,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="119"/>
+      <c r="BE21" s="130"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>Belgium</v>
@@ -32811,7 +32812,7 @@
       <c r="BS21" s="25"/>
       <c r="BT21" s="25"/>
     </row>
-    <row r="22" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>16</v>
       </c>
@@ -32977,7 +32978,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="118">
+      <c r="AY22" s="129">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33010,7 +33011,7 @@
       <c r="BS22" s="25"/>
       <c r="BT22" s="35"/>
     </row>
-    <row r="23" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>17</v>
       </c>
@@ -33176,7 +33177,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="119"/>
+      <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>Japan</v>
@@ -33199,19 +33200,19 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="118">
+      <c r="BQ23" s="129">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
         <f>T76</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="BS23" s="29">
         <v>1</v>
       </c>
       <c r="BT23" s="30"/>
     </row>
-    <row r="24" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>18</v>
       </c>
@@ -33374,7 +33375,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="119"/>
+      <c r="BQ24" s="130"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>Spain</v>
@@ -33384,7 +33385,7 @@
       </c>
       <c r="BT24" s="33"/>
     </row>
-    <row r="25" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>19</v>
       </c>
@@ -33487,7 +33488,7 @@
       <c r="BS25" s="25"/>
       <c r="BT25" s="25"/>
     </row>
-    <row r="26" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>20</v>
       </c>
@@ -33657,7 +33658,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="129">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33687,7 +33688,7 @@
       <c r="BS26" s="25"/>
       <c r="BT26" s="25"/>
     </row>
-    <row r="27" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>21</v>
       </c>
@@ -33857,7 +33858,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="119"/>
+      <c r="AY27" s="130"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>Russia</v>
@@ -33888,7 +33889,7 @@
       <c r="BS27" s="25"/>
       <c r="BT27" s="25"/>
     </row>
-    <row r="28" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>22</v>
       </c>
@@ -34060,7 +34061,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="118">
+      <c r="BE28" s="129">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34084,7 +34085,7 @@
       <c r="BS28" s="25"/>
       <c r="BT28" s="25"/>
     </row>
-    <row r="29" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>23</v>
       </c>
@@ -34259,7 +34260,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="119"/>
+      <c r="BE29" s="130"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>Croatia</v>
@@ -34281,7 +34282,7 @@
       <c r="BS29" s="25"/>
       <c r="BT29" s="25"/>
     </row>
-    <row r="30" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>24</v>
       </c>
@@ -34427,7 +34428,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="118">
+      <c r="AY30" s="129">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34457,7 +34458,7 @@
       <c r="BS30" s="25"/>
       <c r="BT30" s="25"/>
     </row>
-    <row r="31" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>25</v>
       </c>
@@ -34527,7 +34528,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="119"/>
+      <c r="AY31" s="130"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>Denmark</v>
@@ -34553,15 +34554,15 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="124" t="str">
+      <c r="BQ31" s="131" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="125"/>
-      <c r="BS31" s="125"/>
-      <c r="BT31" s="126"/>
+      <c r="BR31" s="132"/>
+      <c r="BS31" s="132"/>
+      <c r="BT31" s="133"/>
     </row>
-    <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>26</v>
       </c>
@@ -34743,7 +34744,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="118">
+      <c r="BK32" s="129">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34756,12 +34757,12 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="127"/>
-      <c r="BR32" s="128"/>
-      <c r="BS32" s="128"/>
-      <c r="BT32" s="129"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="135"/>
+      <c r="BS32" s="135"/>
+      <c r="BT32" s="136"/>
     </row>
-    <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>27</v>
       </c>
@@ -34946,10 +34947,10 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="119"/>
+      <c r="BK33" s="130"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
       <c r="BM33" s="32">
         <v>0</v>
@@ -34962,7 +34963,7 @@
       <c r="BS33" s="25"/>
       <c r="BT33" s="25"/>
     </row>
-    <row r="34" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>28</v>
       </c>
@@ -35128,7 +35129,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="118">
+      <c r="AY34" s="129">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35161,7 +35162,7 @@
       <c r="BS34" s="25"/>
       <c r="BT34" s="35"/>
     </row>
-    <row r="35" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>29</v>
       </c>
@@ -35327,7 +35328,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="119"/>
+      <c r="AY35" s="130"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>Switzerland</v>
@@ -35353,7 +35354,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="118">
+      <c r="BQ35" s="129">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35365,7 +35366,7 @@
       </c>
       <c r="BT35" s="30"/>
     </row>
-    <row r="36" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>30</v>
       </c>
@@ -35517,7 +35518,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="118">
+      <c r="BE36" s="129">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -35525,7 +35526,7 @@
         <v>Sweden</v>
       </c>
       <c r="BG36" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH36" s="30"/>
       <c r="BI36" s="40"/>
@@ -35536,17 +35537,17 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="119"/>
+      <c r="BQ36" s="130"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
       <c r="BS36" s="32">
         <v>0</v>
       </c>
       <c r="BT36" s="33"/>
     </row>
-    <row r="37" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>31</v>
       </c>
@@ -35625,13 +35626,13 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="119"/>
+      <c r="BE37" s="130"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>Colombia</v>
       </c>
       <c r="BG37" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH37" s="33"/>
       <c r="BI37" s="25"/>
@@ -35647,7 +35648,7 @@
       <c r="BS37" s="25"/>
       <c r="BT37" s="25"/>
     </row>
-    <row r="38" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>32</v>
       </c>
@@ -35817,7 +35818,7 @@
         <f>AR38-AS38</f>
         <v>0</v>
       </c>
-      <c r="AY38" s="118">
+      <c r="AY38" s="129">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35843,7 +35844,7 @@
       <c r="BS38" s="25"/>
       <c r="BT38" s="25"/>
     </row>
-    <row r="39" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>33</v>
       </c>
@@ -36013,7 +36014,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="119"/>
+      <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>England</v>
@@ -36035,7 +36036,7 @@
       <c r="BS39" s="25"/>
       <c r="BT39" s="25"/>
     </row>
-    <row r="40" spans="1:72" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:72" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>34</v>
       </c>
@@ -36202,7 +36203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>35</v>
       </c>
@@ -36368,25 +36369,25 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="120" t="str">
+      <c r="BJ41" s="146" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="120"/>
-      <c r="BL41" s="120"/>
-      <c r="BM41" s="120"/>
-      <c r="BN41" s="120"/>
-      <c r="BO41" s="122" t="str">
+      <c r="BK41" s="146"/>
+      <c r="BL41" s="146"/>
+      <c r="BM41" s="146"/>
+      <c r="BN41" s="146"/>
+      <c r="BO41" s="148" t="str">
         <f>S85</f>
-        <v>Portugal</v>
-      </c>
-      <c r="BP41" s="122"/>
-      <c r="BQ41" s="122"/>
-      <c r="BR41" s="122"/>
-      <c r="BS41" s="122"/>
-      <c r="BT41" s="122"/>
+        <v>France</v>
+      </c>
+      <c r="BP41" s="148"/>
+      <c r="BQ41" s="148"/>
+      <c r="BR41" s="148"/>
+      <c r="BS41" s="148"/>
+      <c r="BT41" s="148"/>
     </row>
-    <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>36</v>
       </c>
@@ -36532,19 +36533,19 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>1</v>
       </c>
-      <c r="BJ42" s="121"/>
-      <c r="BK42" s="121"/>
-      <c r="BL42" s="121"/>
-      <c r="BM42" s="121"/>
-      <c r="BN42" s="121"/>
-      <c r="BO42" s="123"/>
-      <c r="BP42" s="123"/>
-      <c r="BQ42" s="123"/>
-      <c r="BR42" s="123"/>
-      <c r="BS42" s="123"/>
-      <c r="BT42" s="123"/>
+      <c r="BJ42" s="147"/>
+      <c r="BK42" s="147"/>
+      <c r="BL42" s="147"/>
+      <c r="BM42" s="147"/>
+      <c r="BN42" s="147"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="149"/>
+      <c r="BS42" s="149"/>
+      <c r="BT42" s="149"/>
     </row>
-    <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <v>37</v>
       </c>
@@ -36616,7 +36617,7 @@
       </c>
       <c r="AY43" s="80"/>
     </row>
-    <row r="44" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>38</v>
       </c>
@@ -36787,7 +36788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>39</v>
       </c>
@@ -36958,7 +36959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>40</v>
       </c>
@@ -37124,14 +37125,14 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="109" t="s">
+      <c r="AY46" s="137" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="110"/>
-      <c r="BA46" s="110"/>
-      <c r="BB46" s="111"/>
+      <c r="AZ46" s="138"/>
+      <c r="BA46" s="138"/>
+      <c r="BB46" s="139"/>
     </row>
-    <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>41</v>
       </c>
@@ -37297,12 +37298,12 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="112"/>
-      <c r="AZ47" s="113"/>
-      <c r="BA47" s="113"/>
-      <c r="BB47" s="114"/>
+      <c r="AY47" s="140"/>
+      <c r="AZ47" s="141"/>
+      <c r="BA47" s="141"/>
+      <c r="BB47" s="142"/>
     </row>
-    <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>42</v>
       </c>
@@ -37448,12 +37449,12 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="112"/>
-      <c r="AZ48" s="113"/>
-      <c r="BA48" s="113"/>
-      <c r="BB48" s="114"/>
+      <c r="AY48" s="140"/>
+      <c r="AZ48" s="141"/>
+      <c r="BA48" s="141"/>
+      <c r="BB48" s="142"/>
     </row>
-    <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>43</v>
       </c>
@@ -37523,12 +37524,12 @@
         <f>MIN(AI44:AI47)</f>
         <v>-9</v>
       </c>
-      <c r="AY49" s="112"/>
-      <c r="AZ49" s="113"/>
-      <c r="BA49" s="113"/>
-      <c r="BB49" s="114"/>
+      <c r="AY49" s="140"/>
+      <c r="AZ49" s="141"/>
+      <c r="BA49" s="141"/>
+      <c r="BB49" s="142"/>
     </row>
-    <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>44</v>
       </c>
@@ -37698,12 +37699,12 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="113"/>
-      <c r="BA50" s="113"/>
-      <c r="BB50" s="114"/>
+      <c r="AY50" s="140"/>
+      <c r="AZ50" s="141"/>
+      <c r="BA50" s="141"/>
+      <c r="BB50" s="142"/>
     </row>
-    <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>45</v>
       </c>
@@ -37873,12 +37874,12 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="112"/>
-      <c r="AZ51" s="113"/>
-      <c r="BA51" s="113"/>
-      <c r="BB51" s="114"/>
+      <c r="AY51" s="140"/>
+      <c r="AZ51" s="141"/>
+      <c r="BA51" s="141"/>
+      <c r="BB51" s="142"/>
     </row>
-    <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>46</v>
       </c>
@@ -38044,12 +38045,12 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="115"/>
-      <c r="AZ52" s="116"/>
-      <c r="BA52" s="116"/>
-      <c r="BB52" s="117"/>
+      <c r="AY52" s="143"/>
+      <c r="AZ52" s="144"/>
+      <c r="BA52" s="144"/>
+      <c r="BB52" s="145"/>
     </row>
-    <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>47</v>
       </c>
@@ -38216,7 +38217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>48</v>
       </c>
@@ -38363,7 +38364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A55" s="49"/>
       <c r="B55" s="50"/>
       <c r="C55" s="49"/>
@@ -38389,9 +38390,9 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="56" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:54" x14ac:dyDescent="0.2">
       <c r="R58" s="58">
         <f>DATE(2018,6,30)+TIME(7,0,0)+gmt_delta</f>
         <v>43281.541666666664</v>
@@ -38405,7 +38406,7 @@
         <v>Portugal</v>
       </c>
     </row>
-    <row r="59" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R59" s="58">
         <f>DATE(2018,6,30)+TIME(3,0,0)+gmt_delta</f>
         <v>43281.375</v>
@@ -38419,7 +38420,7 @@
         <v>France</v>
       </c>
     </row>
-    <row r="60" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R60" s="58">
         <f>DATE(2018,7,1)+TIME(3,0,0)+gmt_delta</f>
         <v>43282.375</v>
@@ -38433,7 +38434,7 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="61" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R61" s="58">
         <f>DATE(2018,7,1)+TIME(7,0,0)+gmt_delta</f>
         <v>43282.541666666664</v>
@@ -38447,7 +38448,7 @@
         <v>Croatia</v>
       </c>
     </row>
-    <row r="62" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R62" s="58">
         <f>DATE(2018,7,2)+TIME(3,0,0)+gmt_delta</f>
         <v>43283.375</v>
@@ -38461,7 +38462,7 @@
         <v>Brazil</v>
       </c>
     </row>
-    <row r="63" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R63" s="58">
         <f>DATE(2018,7,2)+TIME(7,0,0)+gmt_delta</f>
         <v>43283.541666666664</v>
@@ -38475,7 +38476,7 @@
         <v>Belgium</v>
       </c>
     </row>
-    <row r="64" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R64" s="58">
         <f>DATE(2018,7,3)+TIME(3,0,0)+gmt_delta</f>
         <v>43284.375</v>
@@ -38489,7 +38490,7 @@
         <v>Sweden</v>
       </c>
     </row>
-    <row r="65" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R65" s="58">
         <f>DATE(2018,7,3)+TIME(7,0,0)+gmt_delta</f>
         <v>43284.541666666664</v>
@@ -38503,24 +38504,24 @@
         <v>Colombia</v>
       </c>
     </row>
-    <row r="66" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R69" s="58">
         <f>DATE(2018,7,6)+TIME(3,0,0)+gmt_delta</f>
         <v>43287.375</v>
       </c>
       <c r="S69" s="65" t="str">
         <f>IF(OR(BG12="",BG13=""),"",IF(BG12&gt;BG13,BF12,IF(BG12&lt;BG13,BF13,IF(OR(BH12="",BH13=""),"draw",IF(BH12&gt;BH13,BF12,IF(BH12&lt;BH13,BF13,"draw"))))))</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="T69" s="65" t="str">
         <f>IF(OR(S69="",S69="draw"),INDEX(T,94,lang),S69)</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
     </row>
-    <row r="70" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R70" s="58">
         <f>DATE(2018,7,6)+TIME(7,0,0)+gmt_delta</f>
         <v>43287.541666666664</v>
@@ -38534,7 +38535,7 @@
         <v>Brazil</v>
       </c>
     </row>
-    <row r="71" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R71" s="58">
         <f>DATE(2018,7,7)+TIME(7,0,0)+gmt_delta</f>
         <v>43288.541666666664</v>
@@ -38548,35 +38549,35 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="72" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R72" s="58">
         <f>DATE(2018,7,7)+TIME(3,0,0)+gmt_delta</f>
         <v>43288.375</v>
       </c>
       <c r="S72" s="65" t="str">
         <f>IF(OR(BG36="",BG37=""),"",IF(BG36&gt;BG37,BF36,IF(BG36&lt;BG37,BF37,IF(OR(BH36="",BH37=""),"draw",IF(BH36&gt;BH37,BF36,IF(BH36&lt;BH37,BF37,"draw"))))))</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
       <c r="T72" s="65" t="str">
         <f>IF(OR(S72="",S72="draw"),INDEX(T,97,lang),S72)</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
     </row>
-    <row r="73" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R76" s="58">
         <f>DATE(2018,7,10)+TIME(7,0,0)+gmt_delta</f>
         <v>43291.541666666664</v>
       </c>
       <c r="S76" s="65" t="str">
         <f>IF(OR(BM16="",BM17=""),"",IF(BM16&gt;BM17,BL16,IF(BM16&lt;BM17,BL17,IF(OR(BN16="",BN17=""),"draw",IF(BN16&gt;BN17,BL16,IF(BN16&lt;BN17,BL17,"draw"))))))</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="T76" s="65" t="str">
         <f>IF(OR(S76="",S76="draw"),INDEX(T,98,lang),S76)</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="U76" s="65" t="str">
         <f>IF(OR(BM16="",BM17=""),"",IF(BM16&lt;BM17,BL16,IF(BM16&gt;BM17,BL17,IF(OR(BN16="",BN17=""),"draw",IF(BN16&lt;BN17,BL16,IF(BN16&gt;BN17,BL17,"draw"))))))</f>
@@ -38587,7 +38588,7 @@
         <v>Brazil</v>
       </c>
     </row>
-    <row r="77" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R77" s="58">
         <f>DATE(2018,7,11)+TIME(7,0,0)+gmt_delta</f>
         <v>43292.541666666664</v>
@@ -38602,16 +38603,16 @@
       </c>
       <c r="U77" s="65" t="str">
         <f>IF(OR(BM32="",BM33=""),"",IF(BM32&lt;BM33,BL32,IF(BM32&gt;BM33,BL33,IF(OR(BN32="",BN33=""),"draw",IF(BN32&lt;BN33,BL32,IF(BN32&gt;BN33,BL33,"draw"))))))</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
       <c r="Z77" s="65" t="str">
         <f>IF(OR(U77="",U77="draw"),INDEX(T,101,lang),U77)</f>
-        <v>Sweden</v>
+        <v>Colombia</v>
       </c>
     </row>
-    <row r="79" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="18:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="18:20" x14ac:dyDescent="0.2">
       <c r="R81" s="58">
         <f>DATE(2018,7,14)+TIME(3,0,0)+gmt_delta</f>
         <v>43295.375</v>
@@ -38621,50 +38622,29 @@
         <v>Brazil</v>
       </c>
     </row>
-    <row r="83" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="18:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="18:20" x14ac:dyDescent="0.2">
       <c r="R85" s="58">
         <f>DATE(2018,7,15)+TIME(4,0,0)+gmt_delta</f>
         <v>43296.416666666664</v>
       </c>
       <c r="S85" s="65" t="str">
         <f>IF(OR(BS23="",BS24=""),"",IF(BS23&gt;BS24,BR23,IF(BS23&lt;BS24,BR24,IF(OR(BT23="",BT24=""),"",IF(BT23&gt;BT24,BR23,IF(BT23&lt;BT24,BR24,""))))))</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
       <c r="T85" s="65" t="str">
         <f>S85</f>
-        <v>Portugal</v>
+        <v>France</v>
       </c>
     </row>
-    <row r="87" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38672,6 +38652,27 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">
@@ -39089,18 +39090,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB10:BB11 BB14:BB15 BB26:BB27 BB30:BB31 BB18:BB19 BB22:BB23 BB34:BB35 BB38:BB39 BH12:BH13 BH20:BH21 BH28:BH29 BH36:BH37 BN16:BN17 BN32:BN33 BT23:BT24 BT35:BT36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB10:BB11 BB14:BB15 BB26:BB27 BB30:BB31 BB18:BB19 BB22:BB23 BB34:BB35 BB38:BB39 BH12:BH13 BH20:BH21 BH28:BH29 BH36:BH37 BN16:BN17 BN32:BN33 BT23:BT24 BT35:BT36" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G55 BA26:BA27 BA10:BA11 BA14:BA15 BA30:BA31 BA18:BA19 BA22:BA23 BA34:BA35 BA38:BA39 BG12:BG13 BG20:BG21 BG28:BG29 BG36:BG37 BM16:BM17 BM32:BM33 BS23:BS24 BS35:BS36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G55 BA26:BA27 BA10:BA11 BA14:BA15 BA30:BA31 BA18:BA19 BA22:BA23 BA34:BA35 BA38:BA39 BG12:BG13 BG20:BG21 BG28:BG29 BG36:BG37 BM16:BM17 BM32:BM33 BS23:BS24 BS35:BS36" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="O3" location="Settings!C4" tooltip="Settings" display="Settings!C4"/>
-    <hyperlink ref="J5:P5" r:id="rId1" tooltip="Excel Schedule" display="Home Page: www.excely.com"/>
-    <hyperlink ref="J5:P6" r:id="rId2" tooltip="World Cup 2018 Schedule in Excel" display="Home Page: www.excely.com"/>
-    <hyperlink ref="AY46:BB52" r:id="rId3" tooltip="FIFA World Cup Historical Data 1930 - 2014" display="http://www.excely.com/football/fifa-world-cup-statistics.shtml"/>
+    <hyperlink ref="O3" location="Settings!C4" tooltip="Settings" display="Settings!C4" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J5:P5" r:id="rId1" tooltip="Excel Schedule" display="Home Page: www.excely.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J5:P6" r:id="rId2" tooltip="World Cup 2018 Schedule in Excel" display="Home Page: www.excely.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="AY46:BB52" r:id="rId3" tooltip="FIFA World Cup Historical Data 1930 - 2014" display="http://www.excely.com/football/fifa-world-cup-statistics.shtml" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>